<commit_message>
Fault localization with FPs detection
</commit_message>
<xml_diff>
--- a/statistics/features.xlsx
+++ b/statistics/features.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="25">
   <si>
     <t>System</t>
   </si>
@@ -30,16 +30,16 @@
     <t>FP</t>
   </si>
   <si>
-    <t>executed_susp_stmt_vs_susp_stmt_in_passing_variant</t>
-  </si>
-  <si>
-    <t>not_executed_susp_stmt_vs_susp_stmt_in_passing_variant</t>
-  </si>
-  <si>
-    <t>executed_susp_stmt_vs_susp_stmt_in_a_failed_execution</t>
-  </si>
-  <si>
-    <t>not_executed_susp_stmt_vs_susp_stmt_in_a_failed_execution</t>
+    <t>executed_susp_stmt_in_passing_variant</t>
+  </si>
+  <si>
+    <t>not_executed_susp_stmt_vs_in_passing_variant</t>
+  </si>
+  <si>
+    <t>executed_susp_stmt_in_a_failed_execution</t>
+  </si>
+  <si>
+    <t>not_executed_susp_stmt_in_a_failed_execution</t>
   </si>
   <si>
     <t>tested_unexpected_behaviors_in_passing_variant_50</t>
@@ -78,7 +78,19 @@
     <t>/Users/thu-trangnguyen/Documents/Research/SPL/BankAccountTP/1Bug/4wise/</t>
   </si>
   <si>
+    <t>/Users/thu-trangnguyen/Documents/Research/SPL/Elevator/1Bug/4wise/</t>
+  </si>
+  <si>
+    <t>/Users/thu-trangnguyen/Documents/Research/SPL/Email/1Bug/4wise/</t>
+  </si>
+  <si>
     <t>/Users/thu-trangnguyen/Documents/Research/SPL/ExamDB/1Bug/4wise/</t>
+  </si>
+  <si>
+    <t>/Users/thu-trangnguyen/Documents/Research/SPL/GPL/1Bug/1wise/</t>
+  </si>
+  <si>
+    <t>/Users/thu-trangnguyen/Documents/Research/SPL/ZipMe/1Bug/2wise/</t>
   </si>
 </sst>
 </file>
@@ -410,7 +422,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AG4"/>
+  <dimension ref="A1:AG8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -581,25 +593,25 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0.27</v>
+        <v>0.24</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0.27</v>
+        <v>0.24</v>
       </c>
       <c r="H3">
-        <v>0.1</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="J3">
         <v>0</v>
       </c>
       <c r="K3">
-        <v>0.26</v>
+        <v>0.22</v>
       </c>
       <c r="L3">
         <v>0.05</v>
@@ -620,22 +632,22 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>0.24</v>
+        <v>0.08</v>
       </c>
       <c r="S3">
-        <v>0.64</v>
+        <v>0.63</v>
       </c>
       <c r="T3">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="U3">
-        <v>0.75</v>
+        <v>0.47</v>
       </c>
       <c r="V3">
         <v>0</v>
       </c>
       <c r="W3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X3">
         <v>0.11</v>
@@ -650,22 +662,22 @@
         <v>0.83</v>
       </c>
       <c r="AB3">
-        <v>0.28</v>
+        <v>0.27</v>
       </c>
       <c r="AC3">
-        <v>0.87</v>
+        <v>0.76</v>
       </c>
       <c r="AD3">
-        <v>0.27</v>
+        <v>0.31</v>
       </c>
       <c r="AE3">
-        <v>0.85</v>
+        <v>0.74</v>
       </c>
       <c r="AF3">
-        <v>0.31</v>
+        <v>0.3</v>
       </c>
       <c r="AG3">
-        <v>0.9</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="4" spans="1:33">
@@ -673,100 +685,504 @@
         <v>20</v>
       </c>
       <c r="B4">
+        <v>0.42</v>
+      </c>
+      <c r="C4">
+        <v>0.76</v>
+      </c>
+      <c r="D4">
+        <v>0.05</v>
+      </c>
+      <c r="E4">
+        <v>0.4</v>
+      </c>
+      <c r="F4">
+        <v>0.05</v>
+      </c>
+      <c r="G4">
+        <v>0.4</v>
+      </c>
+      <c r="H4">
+        <v>0.66</v>
+      </c>
+      <c r="I4">
+        <v>0.24</v>
+      </c>
+      <c r="J4">
+        <v>0.06</v>
+      </c>
+      <c r="K4">
+        <v>0.34</v>
+      </c>
+      <c r="L4">
+        <v>0.01</v>
+      </c>
+      <c r="M4">
+        <v>0.34</v>
+      </c>
+      <c r="N4">
+        <v>0.3</v>
+      </c>
+      <c r="O4">
+        <v>0.47</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0.32</v>
+      </c>
+      <c r="S4">
+        <v>0.62</v>
+      </c>
+      <c r="T4">
+        <v>0.11</v>
+      </c>
+      <c r="U4">
+        <v>0.42</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0.22</v>
+      </c>
+      <c r="Y4">
+        <v>0.79</v>
+      </c>
+      <c r="Z4">
+        <v>0.27</v>
+      </c>
+      <c r="AA4">
+        <v>0.79</v>
+      </c>
+      <c r="AB4">
+        <v>0.31</v>
+      </c>
+      <c r="AC4">
+        <v>0.7</v>
+      </c>
+      <c r="AD4">
+        <v>0.26</v>
+      </c>
+      <c r="AE4">
+        <v>0.71</v>
+      </c>
+      <c r="AF4">
+        <v>0.28</v>
+      </c>
+      <c r="AG4">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>0.5</v>
+      </c>
+      <c r="C5">
+        <v>0.55</v>
+      </c>
+      <c r="D5">
+        <v>0.01</v>
+      </c>
+      <c r="E5">
+        <v>0.38</v>
+      </c>
+      <c r="F5">
+        <v>0.01</v>
+      </c>
+      <c r="G5">
+        <v>0.38</v>
+      </c>
+      <c r="H5">
+        <v>0.84</v>
+      </c>
+      <c r="I5">
+        <v>0.29</v>
+      </c>
+      <c r="J5">
+        <v>0.01</v>
+      </c>
+      <c r="K5">
+        <v>0.34</v>
+      </c>
+      <c r="L5">
+        <v>0.04</v>
+      </c>
+      <c r="M5">
+        <v>0.35</v>
+      </c>
+      <c r="N5">
+        <v>0.05</v>
+      </c>
+      <c r="O5">
+        <v>0.43</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0.44</v>
+      </c>
+      <c r="S5">
+        <v>0.45</v>
+      </c>
+      <c r="T5">
+        <v>0.23</v>
+      </c>
+      <c r="U5">
+        <v>0.22</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0.18</v>
+      </c>
+      <c r="Y5">
+        <v>0.88</v>
+      </c>
+      <c r="Z5">
+        <v>0.34</v>
+      </c>
+      <c r="AA5">
+        <v>0.75</v>
+      </c>
+      <c r="AB5">
+        <v>0.47</v>
+      </c>
+      <c r="AC5">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="AD5">
+        <v>0.76</v>
+      </c>
+      <c r="AE5">
+        <v>0.66</v>
+      </c>
+      <c r="AF5">
+        <v>0.57</v>
+      </c>
+      <c r="AG5">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
         <v>0.49</v>
       </c>
-      <c r="C4">
+      <c r="C6">
         <v>0.54</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0.2</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0.2</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0.22</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0.09</v>
+      </c>
+      <c r="N6">
+        <v>0.02</v>
+      </c>
+      <c r="O6">
+        <v>0.34</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0.44</v>
+      </c>
+      <c r="S6">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0.51</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0.04</v>
+      </c>
+      <c r="Y6">
+        <v>0.96</v>
+      </c>
+      <c r="Z6">
+        <v>0.08</v>
+      </c>
+      <c r="AA6">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="AB6">
+        <v>0.35</v>
+      </c>
+      <c r="AC6">
+        <v>0.75</v>
+      </c>
+      <c r="AD6">
+        <v>0.27</v>
+      </c>
+      <c r="AE6">
+        <v>0.84</v>
+      </c>
+      <c r="AF6">
+        <v>0.33</v>
+      </c>
+      <c r="AG6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7">
+        <v>0.45</v>
+      </c>
+      <c r="C7">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0.09</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0.09</v>
+      </c>
+      <c r="H7">
+        <v>0.86</v>
+      </c>
+      <c r="I7">
+        <v>0.08</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0.09</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0.29</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0.03</v>
+      </c>
+      <c r="S7">
+        <v>0.26</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0.11</v>
+      </c>
+      <c r="Y7">
+        <v>0.92</v>
+      </c>
+      <c r="Z7">
+        <v>0.22</v>
+      </c>
+      <c r="AA7">
+        <v>0.89</v>
+      </c>
+      <c r="AB7">
+        <v>0.25</v>
+      </c>
+      <c r="AC7">
+        <v>0.98</v>
+      </c>
+      <c r="AD7">
         <v>0.23</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0.23</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0.23</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
+      <c r="AE7">
+        <v>0.95</v>
+      </c>
+      <c r="AF7">
+        <v>0.24</v>
+      </c>
+      <c r="AG7">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8">
+        <v>0.32</v>
+      </c>
+      <c r="C8">
+        <v>0.71</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="H8">
+        <v>0.85</v>
+      </c>
+      <c r="I8">
+        <v>0.24</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0.67</v>
+      </c>
+      <c r="L8">
+        <v>0.05</v>
+      </c>
+      <c r="M8">
+        <v>0.19</v>
+      </c>
+      <c r="N8">
         <v>0.09</v>
       </c>
-      <c r="N4">
-        <v>0.02</v>
-      </c>
-      <c r="O4">
+      <c r="O8">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
         <v>0.34</v>
       </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0.83</v>
-      </c>
-      <c r="S4">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="T4">
-        <v>0.8</v>
-      </c>
-      <c r="U4">
-        <v>0.23</v>
-      </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <v>1</v>
-      </c>
-      <c r="X4">
+      <c r="S8">
+        <v>0.63</v>
+      </c>
+      <c r="T8">
         <v>0.04</v>
       </c>
-      <c r="Y4">
-        <v>0.96</v>
-      </c>
-      <c r="Z4">
-        <v>0.08</v>
-      </c>
-      <c r="AA4">
-        <v>0.9399999999999999</v>
-      </c>
-      <c r="AB4">
-        <v>0.22</v>
-      </c>
-      <c r="AC4">
-        <v>0.89</v>
-      </c>
-      <c r="AD4">
-        <v>0.14</v>
-      </c>
-      <c r="AE4">
-        <v>0.89</v>
-      </c>
-      <c r="AF4">
-        <v>0.21</v>
-      </c>
-      <c r="AG4">
+      <c r="U8">
+        <v>0.46</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>0.1</v>
+      </c>
+      <c r="Y8">
         <v>0.92</v>
+      </c>
+      <c r="Z8">
+        <v>0.29</v>
+      </c>
+      <c r="AA8">
+        <v>0.92</v>
+      </c>
+      <c r="AB8">
+        <v>0.52</v>
+      </c>
+      <c r="AC8">
+        <v>0.66</v>
+      </c>
+      <c r="AD8">
+        <v>0.2</v>
+      </c>
+      <c r="AE8">
+        <v>0.68</v>
+      </c>
+      <c r="AF8">
+        <v>0.25</v>
+      </c>
+      <c r="AG8">
+        <v>0.74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>